<commit_message>
PCB REV B0 * Fix STC3100 grounding * Make R16,R17 DNP by default * Bump Bot Silk to REVB0
</commit_message>
<xml_diff>
--- a/fab/loRaWan1262_jlc-top-pos.xlsx
+++ b/fab/loRaWan1262_jlc-top-pos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ec6aaaf25507da9/Documents/KICAD/loRaWan1262_jlc/gerb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ec6aaaf25507da9/Documents/KICAD/loRaWan1262_jlc/fab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73C99281-1355-4EFB-87C0-33A04F83E454}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48578F7A-FF0A-428C-B771-3733FE28D465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276"/>
   </bookViews>
@@ -1103,10 +1103,17 @@
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.53125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
PCB REV C0 * Make U8 footprint capable of crypto and fram device * Minor updates to schematic * Minor updates to doc prints * Update bot silk to REV C0
</commit_message>
<xml_diff>
--- a/fab/loRaWan1262_jlc-top-pos.xlsx
+++ b/fab/loRaWan1262_jlc-top-pos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ec6aaaf25507da9/Documents/KICAD/loRaWan1262_jlc/fab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48578F7A-FF0A-428C-B771-3733FE28D465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB6565F8-0E43-4282-89FD-6AB55EE8023A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276"/>
   </bookViews>
@@ -22,6 +22,21 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="80">
   <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Mid X</t>
+  </si>
+  <si>
+    <t>Mid Y</t>
+  </si>
+  <si>
+    <t>Layer</t>
+  </si>
+  <si>
+    <t>Rotation</t>
+  </si>
+  <si>
     <t>C1</t>
   </si>
   <si>
@@ -245,21 +260,6 @@
   </si>
   <si>
     <t>Y2</t>
-  </si>
-  <si>
-    <t>Designator</t>
-  </si>
-  <si>
-    <t>Mid X</t>
-  </si>
-  <si>
-    <t>Mid Y</t>
-  </si>
-  <si>
-    <t>Layer</t>
-  </si>
-  <si>
-    <t>Rotation</t>
   </si>
 </sst>
 </file>
@@ -1102,39 +1102,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.53125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>122.8344</v>
@@ -1143,7 +1134,7 @@
         <v>-94.932500000000005</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1151,7 +1142,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>122.8344</v>
@@ -1160,7 +1151,7 @@
         <v>-97.028000000000006</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>180</v>
@@ -1168,7 +1159,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>128.524</v>
@@ -1177,7 +1168,7 @@
         <v>-86.5886</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <v>270</v>
@@ -1185,7 +1176,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>169.60849999999999</v>
@@ -1194,7 +1185,7 @@
         <v>-83.248500000000007</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>180</v>
@@ -1202,7 +1193,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>141.732</v>
@@ -1211,7 +1202,7 @@
         <v>-81.534000000000006</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <v>180</v>
@@ -1219,7 +1210,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>137.79499999999999</v>
@@ -1228,7 +1219,7 @@
         <v>-84.391499999999994</v>
       </c>
       <c r="D7" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <v>90</v>
@@ -1236,7 +1227,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>135.38200000000001</v>
@@ -1245,7 +1236,7 @@
         <v>-95.8215</v>
       </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1253,7 +1244,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>133.477</v>
@@ -1262,7 +1253,7 @@
         <v>-95.8215</v>
       </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1270,7 +1261,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>132.77850000000001</v>
@@ -1279,7 +1270,7 @@
         <v>-91.058999999999997</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E10">
         <v>180</v>
@@ -1287,7 +1278,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>126.619</v>
@@ -1296,7 +1287,7 @@
         <v>-94.995999999999995</v>
       </c>
       <c r="D11" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E11">
         <v>180</v>
@@ -1304,7 +1295,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>124.714</v>
@@ -1313,7 +1304,7 @@
         <v>-94.995999999999995</v>
       </c>
       <c r="D12" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <v>180</v>
@@ -1321,7 +1312,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>173.0248</v>
@@ -1330,7 +1321,7 @@
         <v>-92.201999999999998</v>
       </c>
       <c r="D13" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E13">
         <v>180</v>
@@ -1338,7 +1329,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>162.43299999999999</v>
@@ -1347,7 +1338,7 @@
         <v>-99.123500000000007</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1355,7 +1346,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>170.33240000000001</v>
@@ -1364,7 +1355,7 @@
         <v>-92.201999999999998</v>
       </c>
       <c r="D15" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>180</v>
@@ -1372,7 +1363,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>161.3535</v>
@@ -1381,7 +1372,7 @@
         <v>-99.100499999999997</v>
       </c>
       <c r="D16" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1389,7 +1380,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>160.71850000000001</v>
@@ -1398,7 +1389,7 @@
         <v>-89.598500000000001</v>
       </c>
       <c r="D17" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E17">
         <v>270</v>
@@ -1406,7 +1397,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>160.7415</v>
@@ -1415,7 +1406,7 @@
         <v>-88.646000000000001</v>
       </c>
       <c r="D18" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E18">
         <v>270</v>
@@ -1423,7 +1414,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>147.47244699999999</v>
@@ -1432,7 +1423,7 @@
         <v>-94.653053</v>
       </c>
       <c r="D19" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E19">
         <v>270</v>
@@ -1440,7 +1431,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>150.68549999999999</v>
@@ -1449,7 +1440,7 @@
         <v>-81.406999999999996</v>
       </c>
       <c r="D20" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E20">
         <v>180</v>
@@ -1457,7 +1448,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B21">
         <v>152.01900000000001</v>
@@ -1466,7 +1457,7 @@
         <v>-94.297499999999999</v>
       </c>
       <c r="D21" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <v>90</v>
@@ -1474,7 +1465,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>169.54499999999999</v>
@@ -1483,7 +1474,7 @@
         <v>-89.090500000000006</v>
       </c>
       <c r="D22" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E22">
         <v>180</v>
@@ -1491,7 +1482,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B23">
         <v>157.226</v>
@@ -1500,7 +1491,7 @@
         <v>-89.956500000000005</v>
       </c>
       <c r="D23" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E23">
         <v>180</v>
@@ -1508,7 +1499,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B24">
         <v>169.54499999999999</v>
@@ -1517,7 +1508,7 @@
         <v>-94.995999999999995</v>
       </c>
       <c r="D24" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1525,7 +1516,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B25">
         <v>153.416</v>
@@ -1534,7 +1525,7 @@
         <v>-95.798500000000004</v>
       </c>
       <c r="D25" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1542,7 +1533,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B26">
         <v>157.16249999999999</v>
@@ -1551,7 +1542,7 @@
         <v>-92.773499999999999</v>
       </c>
       <c r="D26" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E26">
         <v>180</v>
@@ -1559,7 +1550,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B27">
         <v>161.16300000000001</v>
@@ -1568,7 +1559,7 @@
         <v>-95.313500000000005</v>
       </c>
       <c r="D27" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E27">
         <v>180</v>
@@ -1576,7 +1567,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B28">
         <v>147.19300000000001</v>
@@ -1585,7 +1576,7 @@
         <v>-96.202500000000001</v>
       </c>
       <c r="D28" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1593,7 +1584,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B29">
         <v>143.82749999999999</v>
@@ -1602,7 +1593,7 @@
         <v>-86.296499999999995</v>
       </c>
       <c r="D29" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E29">
         <v>180</v>
@@ -1610,7 +1601,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B30">
         <v>152.3365</v>
@@ -1619,7 +1610,7 @@
         <v>-96.202500000000001</v>
       </c>
       <c r="D30" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1627,7 +1618,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B31">
         <v>158.75</v>
@@ -1636,7 +1627,7 @@
         <v>-89.979500000000002</v>
       </c>
       <c r="D31" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E31">
         <v>180</v>
@@ -1644,7 +1635,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B32">
         <v>125.491</v>
@@ -1653,7 +1644,7 @@
         <v>-91.947999999999993</v>
       </c>
       <c r="D32" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E32">
         <v>90</v>
@@ -1661,7 +1652,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B33">
         <v>125.857</v>
@@ -1670,7 +1661,7 @@
         <v>-89.027000000000001</v>
       </c>
       <c r="D33" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E33">
         <v>90</v>
@@ -1678,7 +1669,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B34">
         <v>130.75919999999999</v>
@@ -1687,7 +1678,7 @@
         <v>-87.604600000000005</v>
       </c>
       <c r="D34" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E34">
         <v>270</v>
@@ -1695,7 +1686,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B35">
         <v>115.95099999999999</v>
@@ -1704,7 +1695,7 @@
         <v>-83.82</v>
       </c>
       <c r="D35" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E35">
         <v>90</v>
@@ -1712,7 +1703,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B36">
         <v>115.95099999999999</v>
@@ -1721,7 +1712,7 @@
         <v>-94.297499999999999</v>
       </c>
       <c r="D36" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E36">
         <v>90</v>
@@ -1729,7 +1720,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B37">
         <v>125.095</v>
@@ -1738,7 +1729,7 @@
         <v>-82.55</v>
       </c>
       <c r="D37" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E37">
         <v>180</v>
@@ -1746,7 +1737,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B38">
         <v>174.4726</v>
@@ -1755,7 +1746,7 @@
         <v>-85.407499999999999</v>
       </c>
       <c r="D38" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E38">
         <v>180</v>
@@ -1763,7 +1754,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B39">
         <v>117.09399999999999</v>
@@ -1772,7 +1763,7 @@
         <v>-89.153999999999996</v>
       </c>
       <c r="D39" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E39">
         <v>270</v>
@@ -1780,7 +1771,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B40">
         <v>129.92099999999999</v>
@@ -1789,7 +1780,7 @@
         <v>-96.266000000000005</v>
       </c>
       <c r="D40" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E40">
         <v>270</v>
@@ -1797,7 +1788,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B41">
         <v>164.846</v>
@@ -1806,7 +1797,7 @@
         <v>-99.123500000000007</v>
       </c>
       <c r="D41" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E41">
         <v>270</v>
@@ -1814,7 +1805,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B42">
         <v>171.62780000000001</v>
@@ -1823,7 +1814,7 @@
         <v>-92.646500000000003</v>
       </c>
       <c r="D42" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E42">
         <v>270</v>
@@ -1831,7 +1822,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B43">
         <v>159.512</v>
@@ -1840,7 +1831,7 @@
         <v>-92.773499999999999</v>
       </c>
       <c r="D43" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E43">
         <v>90</v>
@@ -1848,7 +1839,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B44">
         <v>121.99850000000001</v>
@@ -1857,7 +1848,7 @@
         <v>-91.947999999999993</v>
       </c>
       <c r="D44" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E44">
         <v>90</v>
@@ -1865,7 +1856,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B45">
         <v>144.7165</v>
@@ -1874,7 +1865,7 @@
         <v>-95.376999999999995</v>
       </c>
       <c r="D45" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1882,7 +1873,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B46">
         <v>118.3005</v>
@@ -1891,7 +1882,7 @@
         <v>-94.932500000000005</v>
       </c>
       <c r="D46" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1899,7 +1890,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B47">
         <v>119.8245</v>
@@ -1908,7 +1899,7 @@
         <v>-82.042000000000002</v>
       </c>
       <c r="D47" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E47">
         <v>180</v>
@@ -1916,7 +1907,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B48">
         <v>131.82599999999999</v>
@@ -1925,7 +1916,7 @@
         <v>-81.915000000000006</v>
       </c>
       <c r="D48" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E48">
         <v>90</v>
@@ -1933,7 +1924,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B49">
         <v>128.524</v>
@@ -1942,7 +1933,7 @@
         <v>-87.5792</v>
       </c>
       <c r="D49" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E49">
         <v>90</v>
@@ -1950,7 +1941,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B50">
         <v>136.017</v>
@@ -1959,7 +1950,7 @@
         <v>-81.953000000000003</v>
       </c>
       <c r="D50" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E50">
         <v>180</v>
@@ -1967,7 +1958,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B51">
         <v>140.08099999999999</v>
@@ -1976,7 +1967,7 @@
         <v>-85.026499999999999</v>
       </c>
       <c r="D51" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -1984,7 +1975,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B52">
         <v>146.304</v>
@@ -1993,7 +1984,7 @@
         <v>-93.662499999999994</v>
       </c>
       <c r="D52" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E52">
         <v>90</v>
@@ -2001,7 +1992,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B53">
         <v>142.43049999999999</v>
@@ -2010,7 +2001,7 @@
         <v>-95.908000000000001</v>
       </c>
       <c r="D53" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E53">
         <v>180</v>
@@ -2018,7 +2009,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B54">
         <v>162.75049999999999</v>
@@ -2027,7 +2018,7 @@
         <v>-83.248500000000007</v>
       </c>
       <c r="D54" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -2035,7 +2026,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B55">
         <v>143.04249999999999</v>
@@ -2044,7 +2035,7 @@
         <v>-93.599000000000004</v>
       </c>
       <c r="D55" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E55">
         <v>270</v>
@@ -2052,7 +2043,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B56">
         <v>132.77850000000001</v>
@@ -2061,7 +2052,7 @@
         <v>-93.090999999999994</v>
       </c>
       <c r="D56" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E56">
         <v>180</v>
@@ -2069,7 +2060,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B57">
         <v>134.59700000000001</v>
@@ -2078,7 +2069,7 @@
         <v>-92.456000000000003</v>
       </c>
       <c r="D57" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E57">
         <v>270</v>
@@ -2086,7 +2077,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B58">
         <v>162.75049999999999</v>
@@ -2095,7 +2086,7 @@
         <v>-89.090500000000006</v>
       </c>
       <c r="D58" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -2103,7 +2094,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B59">
         <v>162.68700000000001</v>
@@ -2112,7 +2103,7 @@
         <v>-95.0595</v>
       </c>
       <c r="D59" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -2120,7 +2111,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B60">
         <v>154.90194700000001</v>
@@ -2129,7 +2120,7 @@
         <v>-92.938552999999999</v>
       </c>
       <c r="D60" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E60">
         <v>135</v>
@@ -2137,7 +2128,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B61">
         <v>136.0805</v>
@@ -2146,7 +2137,7 @@
         <v>-88.138000000000005</v>
       </c>
       <c r="D61" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -2154,7 +2145,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B62">
         <v>136.0805</v>
@@ -2163,7 +2154,7 @@
         <v>-89.915999999999997</v>
       </c>
       <c r="D62" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E62">
         <v>180</v>
@@ -2171,7 +2162,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B63">
         <v>142.1765</v>
@@ -2180,7 +2171,7 @@
         <v>-85.026499999999999</v>
       </c>
       <c r="D63" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -2188,7 +2179,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B64">
         <v>141.09700000000001</v>
@@ -2197,7 +2188,7 @@
         <v>-85.026499999999999</v>
       </c>
       <c r="D64" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -2205,7 +2196,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B65">
         <v>120.5865</v>
@@ -2214,7 +2205,7 @@
         <v>-96.138999999999996</v>
       </c>
       <c r="D65" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -2222,7 +2213,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B66">
         <v>133.0198</v>
@@ -2231,7 +2222,7 @@
         <v>-85.216999999999999</v>
       </c>
       <c r="D66" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E66">
         <v>180</v>
@@ -2239,7 +2230,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B67">
         <v>139.00149999999999</v>
@@ -2248,7 +2239,7 @@
         <v>-82.168999999999997</v>
       </c>
       <c r="D67" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E67">
         <v>270</v>
@@ -2256,7 +2247,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B68">
         <v>138.7475</v>
@@ -2265,7 +2256,7 @@
         <v>-95.25</v>
       </c>
       <c r="D68" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -2273,7 +2264,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B69">
         <v>138.7475</v>
@@ -2282,7 +2273,7 @@
         <v>-91.503500000000003</v>
       </c>
       <c r="D69" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -2290,7 +2281,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B70">
         <v>129.9845</v>
@@ -2299,7 +2290,7 @@
         <v>-92.392499999999998</v>
       </c>
       <c r="D70" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E70">
         <v>180</v>
@@ -2307,7 +2298,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B71">
         <v>159.32149999999999</v>
@@ -2316,15 +2307,15 @@
         <v>-84.454999999999998</v>
       </c>
       <c r="D71" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E71">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B72">
         <v>150.62200000000001</v>
@@ -2333,7 +2324,7 @@
         <v>-87.884</v>
       </c>
       <c r="D72" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E72">
         <v>45</v>
@@ -2341,7 +2332,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B73">
         <v>122.55500000000001</v>
@@ -2350,7 +2341,7 @@
         <v>-89.027000000000001</v>
       </c>
       <c r="D73" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E73">
         <v>270</v>
@@ -2358,7 +2349,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B74">
         <v>157.300431</v>
@@ -2367,7 +2358,7 @@
         <v>-95.768930999999995</v>
       </c>
       <c r="D74" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E74">
         <v>90</v>
@@ -2375,7 +2366,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B75">
         <v>149.75299999999999</v>
@@ -2384,7 +2375,7 @@
         <v>-96.202500000000001</v>
       </c>
       <c r="D75" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E75">
         <v>90</v>

</xml_diff>